<commit_message>
Alloy model, new use cases
</commit_message>
<xml_diff>
--- a/RASD/Use Case specification 0.1.xlsx
+++ b/RASD/Use Case specification 0.1.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4395" yWindow="645" windowWidth="16590" windowHeight="8415"/>
+    <workbookView xWindow="4395" yWindow="645" windowWidth="16590" windowHeight="8415" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="UC-01" sheetId="1" r:id="rId1"/>
     <sheet name="UC-02" sheetId="3" r:id="rId2"/>
-    <sheet name="UC-03" sheetId="4" r:id="rId3"/>
-    <sheet name="UC-04" sheetId="5" r:id="rId4"/>
-    <sheet name="UC-05" sheetId="6" r:id="rId5"/>
+    <sheet name="UC-03" sheetId="7" r:id="rId3"/>
+    <sheet name="UC-04" sheetId="8" r:id="rId4"/>
+    <sheet name="UC-05" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="74">
   <si>
     <t>No.</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>Name:</t>
-  </si>
-  <si>
-    <t>Related requirements</t>
   </si>
   <si>
     <t>Involved actors</t>
@@ -349,13 +346,7 @@
     <t>Cancel accepted request (passenger)</t>
   </si>
   <si>
-    <t>Cancel accepted request (taxi driver)</t>
-  </si>
-  <si>
     <t>Create account</t>
-  </si>
-  <si>
-    <t>Authenticate</t>
   </si>
   <si>
     <t>A ride is cancelled or there was no ride to cancel</t>
@@ -425,12 +416,177 @@
   <si>
     <t>Processes the request.</t>
   </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Notifies the passenger that his/her request has been deleted.</t>
+  </si>
+  <si>
+    <t>Deletes the request.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select the request he want to cancel and press the button </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Delete.</t>
+    </r>
+  </si>
+  <si>
+    <t>The taxi driver has no more to extinguish that request.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The taxi driver must be logged in the system.
+The taxi driver has already accepted a request.
+Developed any problem so the taxi driver has to cancel the request.
+The taxi driver has launched the MyTaxiService mobile application.
+The taxi driver selects the option </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cancel accepted request</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>3.1. The received information is not correct or complete:
+- The system informs the taxi driver that the sent information is wrong or incomplete.
+- Return to step 1.</t>
+  </si>
+  <si>
+    <t>Creates the taxi driver account in the MyTaxiService mobile appplication and shows the details of the registration with all the information the taxi driver has issued to Milano city.</t>
+  </si>
+  <si>
+    <t>Checks if the username isn't already in use, that the password is valid and if the registration code is right.</t>
+  </si>
+  <si>
+    <t>Replies the system with a new username, the password and the registration code.</t>
+  </si>
+  <si>
+    <t>Asks the taxi driver to choose a new username, the password and the registration code.</t>
+  </si>
+  <si>
+    <t>The taxi driver is logged in the MyTaxiService mobile application.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The taxi driver is not registered in MyTaxiService yet.
+The taxi driver has received from Milano city a registration code.
+The taxi driver has launched the MyTaxiService mobile application.
+The taxi driver selects the option </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Create account</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cancel accepted request (taxi driver)</t>
+  </si>
+  <si>
+    <t>Authenticate</t>
+  </si>
+  <si>
+    <t>Related goals</t>
+  </si>
+  <si>
+    <t>S1, S2, S3</t>
+  </si>
+  <si>
+    <t>G1, G3, G5, G6</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2, G3</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The taxi driver is already registered in MyTaxiService.
+The taxi driver has not logged in MyTaxiService yet.
+The taxi driver has launched the MyTaxiService mobile application.
+The taxi driver selects the option </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Log in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Asks the taxi driver his username and password.</t>
+  </si>
+  <si>
+    <t>Replies the system with his username and password.</t>
+  </si>
+  <si>
+    <t>Checks that received information is complete and correct.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -617,6 +773,10 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1187,10 +1347,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1254,6 +1415,55 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1290,16 +1500,8 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1355,15 +1557,11 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1373,6 +1571,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1418,27 +1628,123 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1748,8 +2054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:F22"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1785,10 +2091,10 @@
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="44"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="10" t="s">
         <v>3</v>
       </c>
@@ -1816,64 +2122,68 @@
       <c r="D6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="51"/>
+      <c r="E6" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="66"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="2:8" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="49"/>
+    <row r="7" spans="2:8" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="62"/>
+      <c r="D7" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="59"/>
+      <c r="F7" s="64"/>
       <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="62"/>
+      <c r="D8" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="59"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="46" t="s">
+      <c r="C9" s="78"/>
+      <c r="D9" s="63" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="59"/>
+      <c r="F9" s="64"/>
+    </row>
+    <row r="10" spans="2:8" s="20" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="48" t="s">
+      <c r="C10" s="74"/>
+      <c r="D10" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="49"/>
-    </row>
-    <row r="10" spans="2:8" s="20" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="46" t="s">
+      <c r="E10" s="72"/>
+      <c r="F10" s="73"/>
+    </row>
+    <row r="11" spans="2:8" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="57"/>
-      <c r="F10" s="58"/>
-    </row>
-    <row r="11" spans="2:8" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="89" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
     </row>
     <row r="12" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
@@ -1883,182 +2193,182 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="60" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="62"/>
+      <c r="B13" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="77"/>
     </row>
     <row r="14" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="70" t="s">
+      <c r="B14" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="68"/>
+      <c r="E14" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="68"/>
+      <c r="G14" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="53"/>
-      <c r="G14" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="40"/>
+      <c r="H14" s="80"/>
     </row>
     <row r="15" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="71"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="40"/>
+      <c r="B15" s="86"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="80"/>
     </row>
     <row r="16" spans="2:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="14">
         <v>1</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="45"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="43"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="60"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="90"/>
     </row>
     <row r="17" spans="2:8" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="21">
         <v>2</v>
       </c>
-      <c r="C17" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="35"/>
+      <c r="C17" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="53"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="54"/>
     </row>
     <row r="18" spans="2:8" s="16" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="14">
         <v>3</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="35"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="53"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="54"/>
     </row>
     <row r="19" spans="2:8" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="21">
         <v>4</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="34"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="35"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="53"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="54"/>
     </row>
     <row r="20" spans="2:8" s="16" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="21">
         <v>5</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="34"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="35"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="53"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="54"/>
     </row>
     <row r="21" spans="2:8" s="16" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="21"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="35"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="53"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="54"/>
     </row>
     <row r="22" spans="2:8" s="16" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="21">
         <v>6</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" s="34"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="35"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="53"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="54"/>
     </row>
     <row r="23" spans="2:8" s="16" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="21">
         <v>7</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="H23" s="35"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="54"/>
     </row>
     <row r="24" spans="2:8" s="16" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="21">
         <v>8</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="34"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="35"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="53"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="54"/>
     </row>
     <row r="25" spans="2:8" s="16" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="21">
         <v>9</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="35"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="53"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="54"/>
     </row>
     <row r="26" spans="2:8" s="16" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="15">
         <v>10</v>
       </c>
-      <c r="C26" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="37"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="38"/>
+      <c r="C26" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="56"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="57"/>
     </row>
     <row r="27" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
@@ -2068,38 +2378,38 @@
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="2:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="67" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="68"/>
-      <c r="D28" s="69"/>
+      <c r="B28" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="83"/>
+      <c r="D28" s="84"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="32"/>
+      <c r="B29" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="50"/>
+      <c r="D29" s="51"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="2:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="32"/>
+      <c r="B30" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="50"/>
+      <c r="D30" s="51"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="2:8" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
+      <c r="B31" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="47"/>
+      <c r="D31" s="48"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
@@ -2126,22 +2436,25 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="C21:D21"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G20:H20"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="B7:C7"/>
@@ -2158,10 +2471,6 @@
     <mergeCell ref="B13:H13"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="G14:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="E26:F26"/>
@@ -2180,6 +2489,7 @@
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="E24:F24"/>
+    <mergeCell ref="B28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2192,7 +2502,7 @@
   <dimension ref="B1:G32"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D7" sqref="D7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2210,7 +2520,7 @@
     <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
@@ -2228,10 +2538,10 @@
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="44"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="10" t="s">
         <v>3</v>
       </c>
@@ -2259,64 +2569,68 @@
       <c r="D6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="51"/>
+      <c r="E6" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="66"/>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="49"/>
+    <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="62"/>
+      <c r="D7" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="59"/>
+      <c r="F7" s="64"/>
       <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="62"/>
+      <c r="D8" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="59"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="73" t="s">
+      <c r="C9" s="92"/>
+      <c r="D9" s="93" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
+    </row>
+    <row r="10" spans="2:7" s="20" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="74" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-    </row>
-    <row r="10" spans="2:7" s="20" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="73" t="s">
+      <c r="C10" s="92"/>
+      <c r="D10" s="94" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="94"/>
+      <c r="F10" s="94"/>
+    </row>
+    <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="75" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-    </row>
-    <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="76" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="77" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
+      <c r="C11" s="95"/>
+      <c r="D11" s="96" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="22"/>
@@ -2326,88 +2640,88 @@
       <c r="F12" s="23"/>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="78" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
+      <c r="B13" s="97" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="97"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="80" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="80"/>
-      <c r="E14" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="81"/>
+      <c r="C14" s="99" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="99"/>
+      <c r="E14" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="100"/>
     </row>
     <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="79"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="82"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="101"/>
     </row>
     <row r="16" spans="2:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="24">
         <v>1</v>
       </c>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="35"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="54"/>
     </row>
     <row r="17" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="25">
         <v>2</v>
       </c>
-      <c r="C17" s="83" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="83"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="35"/>
+      <c r="C17" s="102" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="102"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="54"/>
     </row>
     <row r="18" spans="2:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="24">
         <v>3</v>
       </c>
-      <c r="C18" s="83"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="35"/>
+      <c r="C18" s="102"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="54"/>
     </row>
     <row r="19" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="25">
         <v>4</v>
       </c>
-      <c r="C19" s="83"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="35"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="102"/>
+      <c r="E19" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="54"/>
     </row>
     <row r="20" spans="2:6" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15">
         <v>5</v>
       </c>
-      <c r="C20" s="84"/>
-      <c r="D20" s="84"/>
-      <c r="E20" s="85" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="86"/>
+      <c r="C20" s="103"/>
+      <c r="D20" s="103"/>
+      <c r="E20" s="104" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="105"/>
     </row>
     <row r="21" spans="2:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="22"/>
@@ -2417,20 +2731,20 @@
       <c r="F21" s="23"/>
     </row>
     <row r="22" spans="2:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="72" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
+      <c r="B22" s="91" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
     </row>
     <row r="23" spans="2:6" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29"/>
+      <c r="B23" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="26"/>
       <c r="F23" s="26"/>
     </row>
@@ -2493,128 +2807,757 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G32"/>
+  <dimension ref="B1:G33"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:F15"/>
+      <selection activeCell="D9" sqref="D9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2" style="16" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="20" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10" style="16" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="17.28515625" style="16"/>
+    <col min="1" max="1" width="2" style="27" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="20" style="27" customWidth="1"/>
+    <col min="5" max="5" width="10" style="27" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="27" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="27" customWidth="1"/>
+    <col min="8" max="16384" width="17.28515625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="B2" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
     </row>
     <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="107"/>
+      <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="41">
         <v>42303</v>
       </c>
-      <c r="G4" s="17"/>
+      <c r="G4" s="30"/>
     </row>
     <row r="5" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="17"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="30"/>
     </row>
     <row r="6" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="12" t="str">
+      <c r="C6" s="37" t="str">
         <f>B2</f>
         <v>UC-03</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="51"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="17"/>
+      <c r="E6" s="108" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="109"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="111"/>
+      <c r="D7" s="112" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="107"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="30"/>
     </row>
     <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="110" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="111"/>
+      <c r="D8" s="112" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="107"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="30"/>
+    </row>
+    <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="17"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="112" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="107"/>
+      <c r="F9" s="113"/>
+    </row>
+    <row r="10" spans="2:7" s="35" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="110" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="115"/>
+      <c r="D10" s="116" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="117"/>
+      <c r="F10" s="118"/>
+    </row>
+    <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="119" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="120"/>
+      <c r="D11" s="121" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="122"/>
+      <c r="F11" s="123"/>
+    </row>
+    <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="31"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+    </row>
+    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="124" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="125"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="125"/>
+      <c r="F13" s="126"/>
+    </row>
+    <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="127" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="129" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="130"/>
+      <c r="E14" s="129" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="131"/>
+    </row>
+    <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="128"/>
+      <c r="C15" s="130"/>
+      <c r="D15" s="130"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="131"/>
+    </row>
+    <row r="16" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="34">
+        <v>1</v>
+      </c>
+      <c r="C16" s="132" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="133"/>
+      <c r="E16" s="132"/>
+      <c r="F16" s="134"/>
+    </row>
+    <row r="17" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="33">
+        <v>2</v>
+      </c>
+      <c r="C17" s="132"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="132" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="134"/>
+    </row>
+    <row r="18" spans="2:6" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="32">
+        <v>3</v>
+      </c>
+      <c r="C18" s="137"/>
+      <c r="D18" s="137"/>
+      <c r="E18" s="137" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="138"/>
+    </row>
+    <row r="19" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="31"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="135" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="125"/>
+      <c r="D20" s="126"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="2:6" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="136" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="122"/>
+      <c r="D21" s="123"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+    </row>
+    <row r="22" spans="2:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="2:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+    </row>
+    <row r="24" spans="2:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+    </row>
+    <row r="25" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+    </row>
+    <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+    </row>
+    <row r="27" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G34"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2" style="27" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="20" style="27" customWidth="1"/>
+    <col min="5" max="5" width="10" style="27" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="27" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="27" customWidth="1"/>
+    <col min="8" max="16384" width="17.28515625" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+    </row>
+    <row r="3" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+    </row>
+    <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="106" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="107"/>
+      <c r="E4" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="41">
+        <v>42303</v>
+      </c>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="5" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="40"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="30"/>
+    </row>
+    <row r="6" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="37" t="str">
+        <f>B2</f>
+        <v>UC-04</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="108" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="109"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="111"/>
+      <c r="D7" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="107"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="30"/>
+    </row>
+    <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="110" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="111"/>
+      <c r="D8" s="112" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="107"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="110" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="114"/>
+      <c r="D9" s="112" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="107"/>
+      <c r="F9" s="113"/>
+    </row>
+    <row r="10" spans="2:7" s="35" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="49"/>
-    </row>
-    <row r="10" spans="2:7" s="20" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="46" t="s">
+      <c r="C10" s="115"/>
+      <c r="D10" s="139" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="140"/>
+      <c r="F10" s="141"/>
+    </row>
+    <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="91"/>
+      <c r="C11" s="120"/>
+      <c r="D11" s="121" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="122"/>
+      <c r="F11" s="123"/>
+    </row>
+    <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="31"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+    </row>
+    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="124" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="125"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="125"/>
+      <c r="F13" s="126"/>
+    </row>
+    <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="127" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="129" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="130"/>
+      <c r="E14" s="129" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="131"/>
+    </row>
+    <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="128"/>
+      <c r="C15" s="130"/>
+      <c r="D15" s="130"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="131"/>
+    </row>
+    <row r="16" spans="2:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="34">
+        <v>1</v>
+      </c>
+      <c r="C16" s="132"/>
+      <c r="D16" s="133"/>
+      <c r="E16" s="132" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="134"/>
+    </row>
+    <row r="17" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="33">
+        <v>2</v>
+      </c>
+      <c r="C17" s="132" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="133"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="134"/>
+    </row>
+    <row r="18" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="33">
+        <v>3</v>
+      </c>
+      <c r="C18" s="132"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="132" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="134"/>
+    </row>
+    <row r="19" spans="2:6" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="32">
+        <v>4</v>
+      </c>
+      <c r="C19" s="137"/>
+      <c r="D19" s="137"/>
+      <c r="E19" s="137" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="138"/>
+    </row>
+    <row r="20" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="31"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="135" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="125"/>
+      <c r="D21" s="126"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+    </row>
+    <row r="22" spans="2:6" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="136" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="122"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="2:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+    </row>
+    <row r="24" spans="2:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+    </row>
+    <row r="25" spans="2:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+    </row>
+    <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+    </row>
+    <row r="27" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+    </row>
+    <row r="28" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2" style="27" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="20" style="27" customWidth="1"/>
+    <col min="5" max="5" width="10" style="27" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="27" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="27" customWidth="1"/>
+    <col min="8" max="16384" width="17.28515625" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+    </row>
+    <row r="3" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+    </row>
+    <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="106" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="107"/>
+      <c r="E4" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="41">
+        <v>42303</v>
+      </c>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="5" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="40"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="30"/>
+    </row>
+    <row r="6" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="37" t="str">
+        <f>B2</f>
+        <v>UC-05</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="108" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="109"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="111"/>
+      <c r="D7" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="107"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="30"/>
+    </row>
+    <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="110" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="111"/>
+      <c r="D8" s="112" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="107"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="30"/>
+    </row>
+    <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="78"/>
+      <c r="D9" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="59"/>
+      <c r="F9" s="64"/>
+    </row>
+    <row r="10" spans="2:7" s="35" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="74"/>
+      <c r="D10" s="71" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="72"/>
+      <c r="F10" s="73"/>
     </row>
     <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
+      <c r="B11" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="88"/>
+      <c r="D11" s="89" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
@@ -2624,119 +3567,136 @@
       <c r="F12" s="17"/>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="87" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="69"/>
+      <c r="B13" s="145" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="84"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="70" t="s">
+      <c r="B14" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="79" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="80"/>
     </row>
     <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="71"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="82"/>
-    </row>
-    <row r="16" spans="2:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="86"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="80"/>
+    </row>
+    <row r="16" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="14">
         <v>1</v>
       </c>
-      <c r="C16" s="88"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="35"/>
-    </row>
-    <row r="17" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="15">
+      <c r="C16" s="146"/>
+      <c r="D16" s="147"/>
+      <c r="E16" s="146" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="148"/>
+    </row>
+    <row r="17" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="21">
         <v>2</v>
       </c>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="38"/>
-    </row>
-    <row r="18" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-    </row>
-    <row r="19" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="67" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="68"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="2:6" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="2:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="2:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="2:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
+      <c r="C17" s="146" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="147"/>
+      <c r="E17" s="146"/>
+      <c r="F17" s="148"/>
+    </row>
+    <row r="18" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="32">
+        <v>3</v>
+      </c>
+      <c r="C18" s="137"/>
+      <c r="D18" s="137"/>
+      <c r="E18" s="137" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="138"/>
+    </row>
+    <row r="19" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="31"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="135" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="125"/>
+      <c r="D20" s="126"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="2:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="142" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="143"/>
+      <c r="D21" s="144"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+    </row>
+    <row r="22" spans="2:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="2:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+    </row>
+    <row r="24" spans="2:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
     </row>
     <row r="25" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+    </row>
+    <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+    </row>
     <row r="27" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="24">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B7:C7"/>
@@ -2749,562 +3709,18 @@
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:F11"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:D15"/>
     <mergeCell ref="E14:F15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="E16:F16"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G32"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="2" style="16" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="20" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10" style="16" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="17.28515625" style="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="19">
-        <v>42303</v>
-      </c>
-      <c r="G4" s="17"/>
-    </row>
-    <row r="5" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="17"/>
-    </row>
-    <row r="6" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="12" t="str">
-        <f>B2</f>
-        <v>UC-04</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="51"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="17"/>
-    </row>
-    <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="49"/>
-    </row>
-    <row r="10" spans="2:7" s="20" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="91"/>
-    </row>
-    <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-    </row>
-    <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-    </row>
-    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="87" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="69"/>
-    </row>
-    <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="70" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="40"/>
-    </row>
-    <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="71"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="40"/>
-    </row>
-    <row r="16" spans="2:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="14">
-        <v>1</v>
-      </c>
-      <c r="C16" s="88"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="35"/>
-    </row>
-    <row r="17" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="15">
-        <v>2</v>
-      </c>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="92"/>
-    </row>
-    <row r="18" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-    </row>
-    <row r="19" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="67" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="68"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="2:6" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="2:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="2:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="2:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G32"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="2" style="16" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="20" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10" style="16" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="17.28515625" style="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="19">
-        <v>42303</v>
-      </c>
-      <c r="G4" s="17"/>
-    </row>
-    <row r="5" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="17"/>
-    </row>
-    <row r="6" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="12" t="str">
-        <f>B2</f>
-        <v>UC-05</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="51"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="17"/>
-    </row>
-    <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="49"/>
-    </row>
-    <row r="10" spans="2:7" s="20" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="91"/>
-    </row>
-    <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-    </row>
-    <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-    </row>
-    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="87" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="69"/>
-    </row>
-    <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="70" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="40"/>
-    </row>
-    <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="71"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="40"/>
-    </row>
-    <row r="16" spans="2:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="14">
-        <v>1</v>
-      </c>
-      <c r="C16" s="88"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="35"/>
-    </row>
-    <row r="17" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="15">
-        <v>2</v>
-      </c>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="92"/>
-    </row>
-    <row r="18" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-    </row>
-    <row r="19" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="67" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="68"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="2:6" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="2:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="2:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="2:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>